<commit_message>
AFDP-256: Change Case Status Approve Process
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-ecm/src/main/resources/rules/drools-form-business-process-rules.xlsx
+++ b/acm-services/acm-service-ecm/src/main/resources/rules/drools-form-business-process-rules.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="580" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="580"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>RuleSet</t>
   </si>
@@ -121,42 +120,26 @@
     <t>complaint</t>
   </si>
   <si>
-    <t>Close Case Request</t>
-  </si>
-  <si>
-    <t>close_case</t>
+    <t>change_case_status</t>
+  </si>
+  <si>
+    <t>Change Case Status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="165"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -223,210 +206,215 @@
     </fill>
   </fills>
   <borders count="12">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="22">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
-  </cellStyleXfs>
-  <cellXfs count="21">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="3" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="4" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="6" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="7" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="8" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -485,36 +473,330 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G23"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E15" activeCellId="0" pane="topLeft" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.515306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.2908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.9030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.6785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.1530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="21.5703125"/>
+    <col min="2" max="2" width="24.28515625"/>
+    <col min="3" max="3" width="49.85546875"/>
+    <col min="4" max="4" width="31.7109375"/>
+    <col min="5" max="5" width="35.7109375"/>
+    <col min="6" max="6" width="24.140625"/>
+    <col min="7" max="7" width="35.5703125"/>
+    <col min="8" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="1"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -524,7 +806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -534,7 +816,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -544,7 +826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="7" t="s">
@@ -554,8 +836,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="6"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
@@ -566,7 +847,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -585,7 +866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -596,7 +877,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="10" t="s">
@@ -615,7 +896,7 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="57.45" outlineLevel="0" r="11">
+    <row r="11" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>16</v>
       </c>
@@ -638,7 +919,7 @@
         <v>22</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="12">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="16" t="s">
         <v>23</v>
@@ -653,7 +934,7 @@
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="16" t="s">
         <v>26</v>
@@ -667,14 +948,14 @@
       <c r="E13" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="19" t="n">
+      <c r="F13" s="19">
         <v>50</v>
       </c>
       <c r="G13" s="19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="16" t="s">
         <v>30</v>
@@ -689,7 +970,7 @@
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="16" t="s">
         <v>32</v>
@@ -704,22 +985,28 @@
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
+      <c r="D16" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="19">
+        <v>50</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="16"/>
       <c r="C17" s="20"/>
@@ -728,7 +1015,7 @@
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="16"/>
       <c r="C18" s="20"/>
@@ -737,7 +1024,7 @@
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="19">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="16"/>
       <c r="C19" s="20"/>
@@ -746,7 +1033,7 @@
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="16"/>
       <c r="C20" s="20"/>
@@ -755,7 +1042,7 @@
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="16"/>
       <c r="C21" s="20"/>
@@ -764,7 +1051,7 @@
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="22">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="16"/>
       <c r="C22" s="20"/>
@@ -773,7 +1060,7 @@
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="16"/>
       <c r="C23" s="20"/>
@@ -783,64 +1070,39 @@
       <c r="G23" s="19"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AFDP-894 - Update all code to upload new files to populate ACM_FILE and ACM_FILE_REVISION tables - Add container name to container table - so we can send the parent name to Solr when content files are indexed
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-ecm/src/main/resources/rules/drools-form-business-process-rules.xlsx
+++ b/acm-services/acm-service-ecm/src/main/resources/rules/drools-form-business-process-rules.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>RuleSet</t>
   </si>
@@ -131,21 +131,16 @@
   </si>
   <si>
     <t>case_file</t>
-  </si>
-  <si>
-    <t>personnelSecurityBackgroundInvestigation</t>
-  </si>
-  <si>
-    <t>P2D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="165"/>
+    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="166"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -339,7 +334,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -421,6 +416,10 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="166" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -504,7 +503,7 @@
   <dimension ref="A2:G23"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F12" activeCellId="0" pane="topLeft" sqref="F12"/>
+      <selection activeCell="G18" activeCellId="0" pane="topLeft" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -737,18 +736,12 @@
       <c r="C17" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="19" t="n">
-        <v>75</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>39</v>
-      </c>
+      <c r="D17" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
       <c r="A18" s="1"/>

</xml_diff>

<commit_message>
Time and Cost approving workflow logic - business process rules
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-ecm/src/main/resources/rules/drools-form-business-process-rules.xlsx
+++ b/acm-services/acm-service-ecm/src/main/resources/rules/drools-form-business-process-rules.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="580" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="580"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
   <si>
     <t>RuleSet</t>
   </si>
@@ -131,39 +130,34 @@
   </si>
   <si>
     <t>case_file</t>
+  </si>
+  <si>
+    <t>Timesheet</t>
+  </si>
+  <si>
+    <t>timesheet</t>
+  </si>
+  <si>
+    <t>Costsheet</t>
+  </si>
+  <si>
+    <t>costsheet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="165"/>
-    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="166"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -224,214 +218,216 @@
     </fill>
   </fills>
   <borders count="12">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
-  </cellStyleXfs>
-  <cellXfs count="22">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="3" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="6" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="7" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="8" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="166" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -490,35 +486,330 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G23"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G18" activeCellId="0" pane="topLeft" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.2908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.8571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.7040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.7091836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.1479591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.5765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.70918367346939"/>
+    <col min="1" max="1" width="21.5703125"/>
+    <col min="2" max="2" width="24.28515625"/>
+    <col min="3" max="3" width="49.85546875"/>
+    <col min="4" max="4" width="31.7109375"/>
+    <col min="5" max="5" width="35.7109375"/>
+    <col min="6" max="6" width="24.140625"/>
+    <col min="7" max="7" width="35.5703125"/>
+    <col min="8" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -528,7 +819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -538,7 +829,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="45" outlineLevel="0" r="4">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -548,7 +839,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="7" t="s">
@@ -558,7 +849,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
@@ -569,7 +860,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -588,7 +879,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -599,7 +890,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="10" t="s">
@@ -618,7 +909,7 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="105" outlineLevel="0" r="11">
+    <row r="11" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>16</v>
       </c>
@@ -641,7 +932,7 @@
         <v>22</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="12">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="16" t="s">
         <v>23</v>
@@ -656,7 +947,7 @@
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="13">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="16" t="s">
         <v>26</v>
@@ -670,14 +961,14 @@
       <c r="E13" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="19" t="n">
+      <c r="F13" s="19">
         <v>50</v>
       </c>
       <c r="G13" s="19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="16" t="s">
         <v>30</v>
@@ -692,7 +983,7 @@
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="16" t="s">
         <v>32</v>
@@ -707,7 +998,7 @@
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="16">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="16" t="s">
         <v>34</v>
@@ -721,14 +1012,14 @@
       <c r="E16" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="19" t="n">
+      <c r="F16" s="19">
         <v>50</v>
       </c>
       <c r="G16" s="19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="16" t="s">
         <v>36</v>
@@ -743,25 +1034,49 @@
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
+      <c r="B18" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="19">
+        <v>50</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="20">
+      <c r="B19" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="19">
+        <v>50</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="16"/>
       <c r="C20" s="20"/>
@@ -770,7 +1085,7 @@
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="21">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="16"/>
       <c r="C21" s="20"/>
@@ -779,7 +1094,7 @@
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="22">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="16"/>
       <c r="C22" s="20"/>
@@ -788,7 +1103,7 @@
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="23">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="16"/>
       <c r="C23" s="20"/>
@@ -798,64 +1113,39 @@
       <c r="G23" s="19"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.70918367346939"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.70918367346939"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>